<commit_message>
Changes before the time windows analysis
End for timeidx was moved to earlier in the script. Paths in the excel were changed.
</commit_message>
<xml_diff>
--- a/cspAnalysis/subsTue.xlsx
+++ b/cspAnalysis/subsTue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20395"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BNPPC08\Desktop\Maria\matlab\Projects\CSP\CSPRepo\cspAnalysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\CSPRepo\cspAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26EDC32-39AA-46F7-BF99-394BE27D1ED9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A208FE-F4C9-4033-AFD4-682B6E0D93E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29295" yWindow="1245" windowWidth="24750" windowHeight="12525" xr2:uid="{D093EC82-0204-41C4-8EFB-4D6BF0B89068}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30630" windowHeight="13470" xr2:uid="{D093EC82-0204-41C4-8EFB-4D6BF0B89068}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
   <si>
     <t>Subnum</t>
   </si>
@@ -69,33 +69,9 @@
     <t>REFTEP_009</t>
   </si>
   <si>
-    <t>P:\2018-12 POSTHOCSOURCE Project\Meshes\Subj2\headmodel.mat</t>
-  </si>
-  <si>
     <t>headmodel</t>
   </si>
   <si>
-    <t>P:\2018-12 POSTHOCSOURCE Project\Meshes\Subj1\headmodel_001.mat</t>
-  </si>
-  <si>
-    <t>P:\2018-12 POSTHOCSOURCE Project\Meshes\Subj4\headmodel_009.mat</t>
-  </si>
-  <si>
-    <t>P:\2018-12 POSTHOCSOURCE Project\Meshes\Subj3\headmodel_016.mat</t>
-  </si>
-  <si>
-    <t>P:\2018-12 POSTHOCSOURCE Project\Meshes\Subj5\headmodel_021.mat</t>
-  </si>
-  <si>
-    <t>P:\2018-12 POSTHOCSOURCE Project\Meshes\Subj7\headmodel_036.mat</t>
-  </si>
-  <si>
-    <t>P:\2018-12 POSTHOCSOURCE Project\Meshes\Subj8\headmodel_059.mat</t>
-  </si>
-  <si>
-    <t>P:\2018-12 POSTHOCSOURCE Project\Meshes\Subj9\headmodel_047.mat</t>
-  </si>
-  <si>
     <t>REFTEP_018</t>
   </si>
   <si>
@@ -132,64 +108,64 @@
     <t>REFTEP_029</t>
   </si>
   <si>
-    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\cspAnalysis\cleaned\sub-019_2.mat</t>
-  </si>
-  <si>
-    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\cspAnalysis\cleaned\sub-018_2.mat</t>
-  </si>
-  <si>
-    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\cspAnalysis\cleaned\sub-021_2.mat</t>
-  </si>
-  <si>
-    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\cspAnalysis\cleaned\sub-023_2.mat</t>
-  </si>
-  <si>
-    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\cspAnalysis\cleaned\sub-024_2.mat</t>
-  </si>
-  <si>
-    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\cspAnalysis\cleaned\sub-020_2.mat</t>
-  </si>
-  <si>
-    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\cspAnalysis\cleaned\sub-022_2.mat</t>
-  </si>
-  <si>
-    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\cspAnalysis\cleaned\sub-025_2.mat</t>
-  </si>
-  <si>
-    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\cspAnalysis\cleaned\sub-026_2.mat</t>
-  </si>
-  <si>
-    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\cspAnalysis\cleaned\sub-027_2.mat</t>
-  </si>
-  <si>
-    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\cspAnalysis\cleaned\sub-028_2.mat</t>
-  </si>
-  <si>
-    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\cspAnalysis\cleaned\sub-029_2.mat</t>
-  </si>
-  <si>
-    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\cspAnalysis\cleaned\sub-001_2.mat</t>
-  </si>
-  <si>
-    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\cspAnalysis\cleaned\sub-002.mat</t>
-  </si>
-  <si>
-    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\cspAnalysis\cleaned\sub-003_2.mat</t>
-  </si>
-  <si>
-    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\cspAnalysis\cleaned\sub-005.mat</t>
-  </si>
-  <si>
-    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\cspAnalysis\cleaned\sub-007.mat</t>
-  </si>
-  <si>
-    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\cspAnalysis\cleaned\sub-008.mat</t>
-  </si>
-  <si>
-    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\cspAnalysis\cleaned\sub-009.mat</t>
-  </si>
-  <si>
-    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\cspAnalysis\cleaned\sub-004.mat</t>
+    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\CSPRepo\cleaned\sub-001_2.mat</t>
+  </si>
+  <si>
+    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\CSPRepo\cleaned\sub-002.mat</t>
+  </si>
+  <si>
+    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\CSPRepo\cleaned\sub-003_2.mat</t>
+  </si>
+  <si>
+    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\CSPRepo\cleaned\sub-004.mat</t>
+  </si>
+  <si>
+    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\CSPRepo\cleaned\sub-005.mat</t>
+  </si>
+  <si>
+    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\CSPRepo\cleaned\sub-007.mat</t>
+  </si>
+  <si>
+    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\CSPRepo\cleaned\sub-008.mat</t>
+  </si>
+  <si>
+    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\CSPRepo\cleaned\sub-009.mat</t>
+  </si>
+  <si>
+    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\CSPRepo\cleaned\sub-018_2.mat</t>
+  </si>
+  <si>
+    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\CSPRepo\cleaned\sub-019_2.mat</t>
+  </si>
+  <si>
+    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\CSPRepo\cleanedsub-020_2.mat</t>
+  </si>
+  <si>
+    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\CSPRepo\cleaned\sub-021_2.mat</t>
+  </si>
+  <si>
+    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\CSPRepo\cleaned\sub-022_2.mat</t>
+  </si>
+  <si>
+    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\CSPRepo\cleaned\sub-023_2.mat</t>
+  </si>
+  <si>
+    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\CSPRepo\cleaned\sub-024_2.mat</t>
+  </si>
+  <si>
+    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\CSPRepo\cleaned\sub-025_2.mat</t>
+  </si>
+  <si>
+    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\CSPRepo\cleaned\sub-026_2.mat</t>
+  </si>
+  <si>
+    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\CSPRepo\cleaned\sub-027_2.mat</t>
+  </si>
+  <si>
+    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\CSPRepo\cleaned\sub-028_2.mat</t>
+  </si>
+  <si>
+    <t>W:\Projects\2018-12 POSTHOCSOURCE Project\analysis_maria\CSPRepo\cleaned\sub-029_2.mat</t>
   </si>
 </sst>
 </file>
@@ -544,7 +520,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,7 +543,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -578,13 +554,10 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -595,13 +568,10 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -612,13 +582,10 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
         <v>4</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -629,13 +596,10 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
         <v>4</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -646,13 +610,10 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
         <v>3</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -663,13 +624,10 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
-      </c>
-      <c r="E7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -680,13 +638,10 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
         <v>4</v>
-      </c>
-      <c r="E8" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -697,13 +652,10 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
         <v>4</v>
-      </c>
-      <c r="E9" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -711,10 +663,10 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s">
         <v>4</v>
@@ -725,10 +677,10 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
         <v>4</v>
@@ -739,10 +691,10 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D12" t="s">
         <v>4</v>
@@ -753,10 +705,10 @@
         <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
         <v>4</v>
@@ -767,10 +719,10 @@
         <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D14" t="s">
         <v>4</v>
@@ -781,10 +733,10 @@
         <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D15" t="s">
         <v>4</v>
@@ -795,10 +747,10 @@
         <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D16" t="s">
         <v>4</v>
@@ -809,7 +761,7 @@
         <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C17" t="s">
         <v>42</v>
@@ -823,7 +775,7 @@
         <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C18" t="s">
         <v>43</v>
@@ -837,7 +789,7 @@
         <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C19" t="s">
         <v>44</v>
@@ -851,7 +803,7 @@
         <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C20" t="s">
         <v>45</v>
@@ -865,7 +817,7 @@
         <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C21" t="s">
         <v>46</v>

</xml_diff>